<commit_message>
fix name Cleaned Tution Fee to Confirm Tution Fee
</commit_message>
<xml_diff>
--- a/data/cleaned_tuition_data.xlsx
+++ b/data/cleaned_tuition_data.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Cleaned Tuition Fee</t>
+          <t>Confirm Tution Fee</t>
         </is>
       </c>
     </row>
@@ -596,10 +596,8 @@
           <t>วศ.บ. สาขาวิชาวิศวกรรมคอมพิวเตอร์</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E5" t="n">
+        <v>17300</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -701,10 +699,8 @@
           <t>วศ.บ. สาขาวิชาวิศวกรรมคอมพิวเตอร์</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E8" t="n">
+        <v>15000</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -2311,10 +2307,8 @@
           <t>วศ.บ. สาขาวิชาวิศวกรรมคอมพิวเตอร์</t>
         </is>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="E54" t="n">
+        <v>40200</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2381,10 +2375,8 @@
           <t>วศ.บ. วิศวกรรมคอมพิวเตอร์และปัญญาประดิษฐ์</t>
         </is>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>_</t>
-        </is>
+      <c r="E56" t="n">
+        <v>45825</v>
       </c>
       <c r="F56" t="inlineStr">
         <is>

</xml_diff>